<commit_message>
add delete from DB
</commit_message>
<xml_diff>
--- a/UsersForRegisteredTest.xlsx
+++ b/UsersForRegisteredTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="35">
   <si>
     <t>email</t>
   </si>
@@ -81,112 +81,49 @@
     <t>community</t>
   </si>
   <si>
-    <t>Petro</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Khrystyna</t>
-  </si>
-  <si>
-    <t>Taras</t>
-  </si>
-  <si>
-    <t>Hluhov</t>
-  </si>
-  <si>
-    <t>Ivanov</t>
-  </si>
-  <si>
-    <t>Rest</t>
-  </si>
-  <si>
-    <t>Soap</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Ivanovych</t>
-  </si>
-  <si>
-    <t>Petrovych</t>
-  </si>
-  <si>
-    <t>Tarasovych</t>
-  </si>
-  <si>
-    <t>Victorovych</t>
-  </si>
-  <si>
-    <t>petro@gmail.com</t>
-  </si>
-  <si>
-    <t>ivan@gmail.com</t>
-  </si>
-  <si>
-    <t>max@gmail.com</t>
-  </si>
-  <si>
-    <t>khrystyna@gmail.com</t>
-  </si>
-  <si>
-    <t>taras@gmail.com</t>
-  </si>
-  <si>
-    <t>khrystyna</t>
-  </si>
-  <si>
-    <t>petro12</t>
-  </si>
-  <si>
-    <t>ivan123</t>
-  </si>
-  <si>
-    <t>max456</t>
-  </si>
-  <si>
-    <t>taras8</t>
-  </si>
-  <si>
     <t>Lviv</t>
   </si>
   <si>
-    <t>Kyiv</t>
-  </si>
-  <si>
-    <t>Ivano-Frankivsk</t>
-  </si>
-  <si>
-    <t>Mkhaylovych</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vinnytsia Oblast</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kharkiv Oblast</t>
-  </si>
-  <si>
-    <t>Dnipropetrovsk Oblast</t>
-  </si>
-  <si>
-    <t>Mykolaiv Oblast</t>
-  </si>
-  <si>
-    <t>Naykova</t>
-  </si>
-  <si>
     <t>СВ</t>
   </si>
   <si>
     <t>Shevchenkivskym</t>
   </si>
   <si>
-    <t>Shevchenkivskym RV</t>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>zzzzz</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>ccccc</t>
+  </si>
+  <si>
+    <t>vvvvv</t>
+  </si>
+  <si>
+    <t>bbbbbb</t>
+  </si>
+  <si>
+    <t>nnnnnnn</t>
+  </si>
+  <si>
+    <t>hhhhhhh</t>
+  </si>
+  <si>
+    <t>ffffff</t>
+  </si>
+  <si>
+    <t>ttttt</t>
+  </si>
+  <si>
+    <t>tttttt</t>
+  </si>
+  <si>
+    <t>email@email.com</t>
   </si>
 </sst>
 </file>
@@ -238,13 +175,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,56 +589,56 @@
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="2">
-        <v>111111</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G2" s="4">
         <v>111111</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="2">
-        <v>32432</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="2">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" s="2">
-        <v>123456</v>
+        <v>21</v>
+      </c>
+      <c r="P2" s="5">
+        <v>111111</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R2" s="2">
+        <v>22</v>
+      </c>
+      <c r="R2" s="5">
         <v>673660000</v>
       </c>
       <c r="S2" s="2" t="s">
@@ -704,56 +647,56 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="2">
-        <v>111111</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G3" s="4">
         <v>111111</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="2">
-        <v>32432</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2">
-        <v>4</v>
-      </c>
-      <c r="M3" s="2">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="2">
-        <v>123456</v>
+        <v>21</v>
+      </c>
+      <c r="P3" s="5">
+        <v>111111</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="2">
+        <v>22</v>
+      </c>
+      <c r="R3" s="5">
         <v>673660000</v>
       </c>
       <c r="S3" s="2" t="s">
@@ -762,56 +705,56 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="2">
-        <v>111111</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G4" s="4">
         <v>111111</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="2">
-        <v>32432</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2">
-        <v>6</v>
-      </c>
-      <c r="M4" s="2">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" s="2">
-        <v>123456</v>
+        <v>21</v>
+      </c>
+      <c r="P4" s="5">
+        <v>111111</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="R4" s="2">
+        <v>22</v>
+      </c>
+      <c r="R4" s="5">
         <v>673660000</v>
       </c>
       <c r="S4" s="2" t="s">
@@ -820,56 +763,56 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2">
-        <v>111111</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G5" s="4">
         <v>111111</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="2">
-        <v>32432</v>
-      </c>
-      <c r="K5" s="1">
-        <v>3</v>
-      </c>
-      <c r="L5" s="2">
-        <v>7</v>
-      </c>
-      <c r="M5" s="2">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" s="2">
-        <v>123456</v>
+        <v>21</v>
+      </c>
+      <c r="P5" s="5">
+        <v>111111</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" s="2">
+        <v>22</v>
+      </c>
+      <c r="R5" s="5">
         <v>673660000</v>
       </c>
       <c r="S5" s="2" t="s">
@@ -878,56 +821,56 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="2">
-        <v>111111</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G6" s="4">
         <v>111111</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="2">
-        <v>32432</v>
-      </c>
-      <c r="K6" s="1">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2">
-        <v>8</v>
-      </c>
-      <c r="M6" s="2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="2">
-        <v>123456</v>
+        <v>21</v>
+      </c>
+      <c r="P6" s="5">
+        <v>111111</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="R6" s="2">
+        <v>22</v>
+      </c>
+      <c r="R6" s="5">
         <v>673660000</v>
       </c>
       <c r="S6" s="2" t="s">
@@ -936,73 +879,293 @@
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G7" s="4">
+        <v>111111</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="5">
+        <v>111111</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="5">
+        <v>673660000</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G8" s="4">
+        <v>111111</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="5">
+        <v>111111</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" s="5">
+        <v>673660000</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="T8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G9" s="4">
+        <v>111111</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="5">
+        <v>111111</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="5">
+        <v>673660000</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G10" s="4">
+        <v>111111</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="O10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="5">
+        <v>111111</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="5">
+        <v>673660000</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4">
+        <v>111111</v>
+      </c>
+      <c r="G11" s="4">
+        <v>111111</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+      <c r="O11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="5">
+        <v>111111</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" s="5">
+        <v>673660000</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="T11" s="2"/>
     </row>
   </sheetData>

</xml_diff>